<commit_message>
update table data in spreadsheet
</commit_message>
<xml_diff>
--- a/source/Assets/BigStarCollectibles CosmosDB.xlsx
+++ b/source/Assets/BigStarCollectibles CosmosDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WR\source\repos\azure-cosmos-db-table-api-2448119\source\Assets\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WR\source\repos\azure-cosmos-db-table-api-2448119\source\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB73AAB1-A5D6-4032-9842-E080BE28EA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B836AC22-7129-4603-98B8-A5BDB3F4A9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1188" yWindow="1188" windowWidth="23040" windowHeight="12612" xr2:uid="{B907D294-0E78-4341-9B43-E726771B09E6}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{B907D294-0E78-4341-9B43-E726771B09E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -862,21 +862,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730AD398-9ECE-4C01-9FCC-52B4D29DF3B8}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
more updates to data
</commit_message>
<xml_diff>
--- a/source/Assets/BigStarCollectibles CosmosDB.xlsx
+++ b/source/Assets/BigStarCollectibles CosmosDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WR\source\repos\azure-cosmos-db-table-api-2448119\source\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B836AC22-7129-4603-98B8-A5BDB3F4A9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158DC83E-A743-4A0B-A10E-C980557B0B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{B907D294-0E78-4341-9B43-E726771B09E6}"/>
+    <workbookView xWindow="31908" yWindow="1188" windowWidth="23040" windowHeight="12612" xr2:uid="{B907D294-0E78-4341-9B43-E726771B09E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -863,7 +863,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1023,7 @@
         <v>23.95</v>
       </c>
       <c r="I10" s="1">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>

</xml_diff>